<commit_message>
Converted JSON to array of array
</commit_message>
<xml_diff>
--- a/applied.xlsx
+++ b/applied.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">REGISTER NO.</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">Abdu Samad M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akshay K S</t>
   </si>
   <si>
     <t xml:space="preserve">TCR15CS008</t>
@@ -159,18 +153,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:D5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -188,7 +182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -202,7 +196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -230,20 +224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Display all, rowsPerPage, Download filtered data
</commit_message>
<xml_diff>
--- a/applied.xlsx
+++ b/applied.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="257">
   <si>
     <t xml:space="preserve">REGISTER NO.</t>
   </si>
@@ -34,40 +34,736 @@
     <t xml:space="preserve">BRANCH</t>
   </si>
   <si>
-    <t xml:space="preserve">IDK15CS039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namitha Murali</t>
+    <t xml:space="preserve">KKE15CH015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashly Williams</t>
   </si>
   <si>
     <t xml:space="preserve">B.Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">Computer Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdu Samad M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anand Simmy Manuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anjali U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anjaly S Menon</t>
+    <t xml:space="preserve">Chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KKE15CH045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reshma T R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhijith R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhiram Kp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adarsh V.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aishwarya P Nambiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleena Shelvi K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amal Haridas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anand Kumar M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anjal Mohammed K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ann Mary John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anwin John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archana Ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun Gopal T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashin V K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashiq Shahul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aswin Muraleedharan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blessmy Rose K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chethan Shyam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dileep Nampoothiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fariz Ismail A R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazil Aziz Abdulla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gayathri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jibin K K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joseph M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jithin M J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiran A S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiran M S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krishnaveni V K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krithya K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumar Namratha Vinaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohammed Unais C P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mona Mangsatabam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammed Shahazad K C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prabhath Ajayakumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pranav Jayaprakash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reethu Mathew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohith R Varier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saroj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sravan K Madhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreekutty K B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve Roy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thawfeequ Rahman Kottukkaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Saji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishnupriya Pp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yadhu Prakash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhil K A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anusha T V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aswathi Vk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CH054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jishnu Pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TKM15CH046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neel Augustine M L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTE15CE038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammed Irfan Kt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTE15CE056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreejith T S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHIJITH ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abin Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achuthan H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aiswarya Menon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajay Krishna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhil P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhil V Sukumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akshaya Patak V.K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anamika K Reghu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anandhu Raj D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anisha N A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anjima C S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anupama Harikumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparna K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archana A R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashique Nisar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashna Francis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athul P K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athulya Mohan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deepak Kumar Mv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dheerajkumar V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godson T Tharakan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gokul Suresh K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gopikrishnan T M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunain K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indu K I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaydeep B Vinod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesty Simon Muttath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karthika M S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khanzah.C.P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.S.NANDHINI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Alfin Terry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mammu Ashif P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manu Varghese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meenu D. Prasad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohammed Akhil Salih</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammed Rashid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammed Arshad U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammed Jasir T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Najma Naurin V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nayana.M.Benoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nihala Mol V.T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nivya Mary Kattissery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prathul Ragesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rashad bin Aboobacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reneesh J Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revathi V V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riyamol Pe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roshan Manesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satheeshkumar S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shilna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinchith M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sooraj T V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourabh Suresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spandhana M Haridas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreehari K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreekesh T K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T R Sreeshna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vandana Purushothaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidhya Raj K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vijitha Vijayan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEBA NAAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashique P A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namitha.P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subhash.K.B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CE095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subin Kundolipurakkal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR15CS013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anupam Asok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science and Engineering</t>
   </si>
   <si>
     <t xml:space="preserve">TCR15CS014</t>
@@ -76,6 +772,9 @@
     <t xml:space="preserve">Aswin Pradeep P</t>
   </si>
   <si>
+    <t xml:space="preserve">CSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCR15CS015</t>
   </si>
   <si>
@@ -92,231 +791,6 @@
   </si>
   <si>
     <t xml:space="preserve">Azra Hashir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digina V P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinusha P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gayathri C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gayathri Devi P A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacob Roy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jashim Gafoor K K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jithin Lal K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jithu J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joel Antony Joy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K Lakshmi Prasad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria Pauly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mohammed Shiyaf Chettali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muneeba Ruby T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohith Krishnan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roshini K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanjay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanjna Mohan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saurav James Zachrias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shreya Davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swarna E M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T S Ajay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiny Mol James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vijitha A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vrindha Viswambharan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vyshnavi Pk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ambili T P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anagha Raveendran R S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aswathi P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarath P K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soumya. M P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subina M T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR15CS072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asha Simon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR17CSCE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aiswarya Roy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M.Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR17CSCE03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asna V.K.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR17CSCE04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bhagyasree P V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR17CSCE05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haritha Madhav C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCR17CSCE06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hasla M</t>
   </si>
 </sst>
 </file>
@@ -414,18 +888,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D122" activeCellId="0" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -485,7 +959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -499,7 +973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
@@ -513,7 +987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
@@ -527,7 +1001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
@@ -541,7 +1015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>20</v>
       </c>
@@ -555,7 +1029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>22</v>
       </c>
@@ -569,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>24</v>
       </c>
@@ -583,7 +1057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>26</v>
       </c>
@@ -597,7 +1071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>28</v>
       </c>
@@ -611,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -625,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>32</v>
       </c>
@@ -639,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>34</v>
       </c>
@@ -653,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>36</v>
       </c>
@@ -667,7 +1141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>38</v>
       </c>
@@ -681,7 +1155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>40</v>
       </c>
@@ -695,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>42</v>
       </c>
@@ -709,7 +1183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>44</v>
       </c>
@@ -723,7 +1197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>46</v>
       </c>
@@ -737,7 +1211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>48</v>
       </c>
@@ -751,7 +1225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>50</v>
       </c>
@@ -765,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>52</v>
       </c>
@@ -779,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>54</v>
       </c>
@@ -793,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>56</v>
       </c>
@@ -807,7 +1281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>58</v>
       </c>
@@ -821,7 +1295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>60</v>
       </c>
@@ -835,7 +1309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>62</v>
       </c>
@@ -849,7 +1323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>64</v>
       </c>
@@ -863,7 +1337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>66</v>
       </c>
@@ -877,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>68</v>
       </c>
@@ -891,7 +1365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>70</v>
       </c>
@@ -905,7 +1379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>72</v>
       </c>
@@ -919,7 +1393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>74</v>
       </c>
@@ -933,7 +1407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>76</v>
       </c>
@@ -947,7 +1421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>78</v>
       </c>
@@ -961,7 +1435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>80</v>
       </c>
@@ -975,7 +1449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>82</v>
       </c>
@@ -989,7 +1463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>84</v>
       </c>
@@ -1003,7 +1477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>86</v>
       </c>
@@ -1017,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>88</v>
       </c>
@@ -1025,63 +1499,63 @@
         <v>89</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="B44" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="B45" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="B46" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="C46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="B47" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="C47" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>7</v>
@@ -1089,10 +1563,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>6</v>
@@ -1103,10 +1577,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>6</v>
@@ -1117,10 +1591,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>6</v>
@@ -1131,10 +1605,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>6</v>
@@ -1145,10 +1619,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>6</v>
@@ -1159,142 +1633,1038 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>7</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>